<commit_message>
Added the conversion between Celsius and Fahrenheit
</commit_message>
<xml_diff>
--- a/Documentation/Gantt_Chart.xlsx
+++ b/Documentation/Gantt_Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{648BC33F-75AD-4593-AFAD-B4B02218F8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45BA945-A4C5-44A1-9892-51A5103686AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>Task 4</t>
   </si>
@@ -213,9 +213,6 @@
     <t>Brenden</t>
   </si>
   <si>
-    <t>Basic CSS addition</t>
-  </si>
-  <si>
     <t>Mid Lab Check-off</t>
   </si>
   <si>
@@ -250,6 +247,21 @@
   </si>
   <si>
     <t>3 hours</t>
+  </si>
+  <si>
+    <t>Conversion Between F/C</t>
+  </si>
+  <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>2.2 hours</t>
+  </si>
+  <si>
+    <t>CSS on HTML Page</t>
+  </si>
+  <si>
+    <t>Next Task</t>
   </si>
 </sst>
 </file>
@@ -824,6 +836,18 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="12">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -831,18 +855,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1409,11 +1421,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL24"/>
+  <dimension ref="A1:BL25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1435,7 +1447,7 @@
         <v>29</v>
       </c>
       <c r="B1" s="53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1449,7 +1461,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I2" s="51"/>
     </row>
@@ -1458,119 +1470,119 @@
         <v>30</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="73">
+      <c r="D3" s="72"/>
+      <c r="E3" s="70">
         <v>44439</v>
       </c>
-      <c r="F3" s="73"/>
+      <c r="F3" s="70"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="72"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="70">
+      <c r="I4" s="67">
         <f>I5</f>
         <v>44438</v>
       </c>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="71"/>
-      <c r="N4" s="71"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="70">
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="67">
         <f>P5</f>
         <v>44445</v>
       </c>
-      <c r="Q4" s="71"/>
-      <c r="R4" s="71"/>
-      <c r="S4" s="71"/>
-      <c r="T4" s="71"/>
-      <c r="U4" s="71"/>
-      <c r="V4" s="72"/>
-      <c r="W4" s="70">
+      <c r="Q4" s="68"/>
+      <c r="R4" s="68"/>
+      <c r="S4" s="68"/>
+      <c r="T4" s="68"/>
+      <c r="U4" s="68"/>
+      <c r="V4" s="69"/>
+      <c r="W4" s="67">
         <f>W5</f>
         <v>44452</v>
       </c>
-      <c r="X4" s="71"/>
-      <c r="Y4" s="71"/>
-      <c r="Z4" s="71"/>
-      <c r="AA4" s="71"/>
-      <c r="AB4" s="71"/>
-      <c r="AC4" s="72"/>
-      <c r="AD4" s="70">
+      <c r="X4" s="68"/>
+      <c r="Y4" s="68"/>
+      <c r="Z4" s="68"/>
+      <c r="AA4" s="68"/>
+      <c r="AB4" s="68"/>
+      <c r="AC4" s="69"/>
+      <c r="AD4" s="67">
         <f>AD5</f>
         <v>44459</v>
       </c>
-      <c r="AE4" s="71"/>
-      <c r="AF4" s="71"/>
-      <c r="AG4" s="71"/>
-      <c r="AH4" s="71"/>
-      <c r="AI4" s="71"/>
-      <c r="AJ4" s="72"/>
-      <c r="AK4" s="70">
+      <c r="AE4" s="68"/>
+      <c r="AF4" s="68"/>
+      <c r="AG4" s="68"/>
+      <c r="AH4" s="68"/>
+      <c r="AI4" s="68"/>
+      <c r="AJ4" s="69"/>
+      <c r="AK4" s="67">
         <f>AK5</f>
         <v>44466</v>
       </c>
-      <c r="AL4" s="71"/>
-      <c r="AM4" s="71"/>
-      <c r="AN4" s="71"/>
-      <c r="AO4" s="71"/>
-      <c r="AP4" s="71"/>
-      <c r="AQ4" s="72"/>
-      <c r="AR4" s="70">
+      <c r="AL4" s="68"/>
+      <c r="AM4" s="68"/>
+      <c r="AN4" s="68"/>
+      <c r="AO4" s="68"/>
+      <c r="AP4" s="68"/>
+      <c r="AQ4" s="69"/>
+      <c r="AR4" s="67">
         <f>AR5</f>
         <v>44473</v>
       </c>
-      <c r="AS4" s="71"/>
-      <c r="AT4" s="71"/>
-      <c r="AU4" s="71"/>
-      <c r="AV4" s="71"/>
-      <c r="AW4" s="71"/>
-      <c r="AX4" s="72"/>
-      <c r="AY4" s="70">
+      <c r="AS4" s="68"/>
+      <c r="AT4" s="68"/>
+      <c r="AU4" s="68"/>
+      <c r="AV4" s="68"/>
+      <c r="AW4" s="68"/>
+      <c r="AX4" s="69"/>
+      <c r="AY4" s="67">
         <f>AY5</f>
         <v>44480</v>
       </c>
-      <c r="AZ4" s="71"/>
-      <c r="BA4" s="71"/>
-      <c r="BB4" s="71"/>
-      <c r="BC4" s="71"/>
-      <c r="BD4" s="71"/>
-      <c r="BE4" s="72"/>
-      <c r="BF4" s="70">
+      <c r="AZ4" s="68"/>
+      <c r="BA4" s="68"/>
+      <c r="BB4" s="68"/>
+      <c r="BC4" s="68"/>
+      <c r="BD4" s="68"/>
+      <c r="BE4" s="69"/>
+      <c r="BF4" s="67">
         <f>BF5</f>
         <v>44487</v>
       </c>
-      <c r="BG4" s="71"/>
-      <c r="BH4" s="71"/>
-      <c r="BI4" s="71"/>
-      <c r="BJ4" s="71"/>
-      <c r="BK4" s="71"/>
-      <c r="BL4" s="72"/>
+      <c r="BG4" s="68"/>
+      <c r="BH4" s="68"/>
+      <c r="BI4" s="68"/>
+      <c r="BJ4" s="68"/>
+      <c r="BK4" s="68"/>
+      <c r="BL4" s="69"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44438</v>
@@ -1816,10 +1828,10 @@
         <v>8</v>
       </c>
       <c r="G6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="I6" s="13" t="str">
         <f t="shared" ref="I6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
@@ -2118,7 +2130,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="59"/>
       <c r="D8" s="19"/>
@@ -2204,10 +2216,10 @@
         <v>44448</v>
       </c>
       <c r="G9" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="56" t="s">
         <v>52</v>
-      </c>
-      <c r="H9" s="56" t="s">
-        <v>53</v>
       </c>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
@@ -2288,10 +2300,10 @@
         <v>44450</v>
       </c>
       <c r="G10" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H10" s="56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
@@ -2370,10 +2382,10 @@
         <v>44451</v>
       </c>
       <c r="G11" s="56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H11" s="56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
@@ -2435,24 +2447,28 @@
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="48"/>
       <c r="B12" s="64" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C12" s="60" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="56">
         <f>F11</f>
         <v>44451</v>
       </c>
       <c r="F12" s="56">
-        <f>E12+1</f>
-        <v>44452</v>
-      </c>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
+        <f>E12</f>
+        <v>44451</v>
+      </c>
+      <c r="G12" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="56" t="s">
+        <v>58</v>
+      </c>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
       <c r="K12" s="34"/>
@@ -2513,12 +2529,21 @@
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="48"/>
       <c r="B13" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="60"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
+        <v>59</v>
+      </c>
+      <c r="C13" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="E13" s="56">
+        <v>44451</v>
+      </c>
+      <c r="F13" s="56">
+        <f>E13</f>
+        <v>44451</v>
+      </c>
       <c r="G13" s="56"/>
       <c r="H13" s="56"/>
       <c r="I13" s="34"/>
@@ -2579,18 +2604,16 @@
       <c r="BL13" s="34"/>
     </row>
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="61"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="60"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
       <c r="K14" s="34"/>
@@ -2649,14 +2672,18 @@
       <c r="BL14" s="34"/>
     </row>
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="49"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
+      <c r="A15" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="61"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
@@ -2715,7 +2742,7 @@
       <c r="BL15" s="34"/>
     </row>
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="48"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="65"/>
       <c r="C16" s="62"/>
       <c r="D16" s="27"/>
@@ -2735,8 +2762,8 @@
       <c r="R16" s="34"/>
       <c r="S16" s="34"/>
       <c r="T16" s="34"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
+      <c r="U16" s="34"/>
+      <c r="V16" s="34"/>
       <c r="W16" s="34"/>
       <c r="X16" s="34"/>
       <c r="Y16" s="34"/>
@@ -2801,8 +2828,8 @@
       <c r="R17" s="34"/>
       <c r="S17" s="34"/>
       <c r="T17" s="34"/>
-      <c r="U17" s="34"/>
-      <c r="V17" s="34"/>
+      <c r="U17" s="35"/>
+      <c r="V17" s="35"/>
       <c r="W17" s="34"/>
       <c r="X17" s="34"/>
       <c r="Y17" s="34"/>
@@ -2848,9 +2875,7 @@
     </row>
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="48"/>
-      <c r="B18" s="65" t="s">
-        <v>0</v>
-      </c>
+      <c r="B18" s="65"/>
       <c r="C18" s="62"/>
       <c r="D18" s="27"/>
       <c r="E18" s="57"/>
@@ -2873,7 +2898,7 @@
       <c r="V18" s="34"/>
       <c r="W18" s="34"/>
       <c r="X18" s="34"/>
-      <c r="Y18" s="35"/>
+      <c r="Y18" s="34"/>
       <c r="Z18" s="34"/>
       <c r="AA18" s="34"/>
       <c r="AB18" s="34"/>
@@ -2917,7 +2942,7 @@
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="48"/>
       <c r="B19" s="65" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="62"/>
       <c r="D19" s="27"/>
@@ -2941,7 +2966,7 @@
       <c r="V19" s="34"/>
       <c r="W19" s="34"/>
       <c r="X19" s="34"/>
-      <c r="Y19" s="34"/>
+      <c r="Y19" s="35"/>
       <c r="Z19" s="34"/>
       <c r="AA19" s="34"/>
       <c r="AB19" s="34"/>
@@ -2983,19 +3008,16 @@
       <c r="BL19" s="34"/>
     </row>
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="66"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17" t="str">
-        <f t="shared" ref="H8:H21" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v/>
-      </c>
+      <c r="A20" s="48"/>
+      <c r="B20" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="62"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
       <c r="K20" s="34"/>
@@ -3054,90 +3076,166 @@
       <c r="BL20" s="34"/>
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="66"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17" t="str">
+        <f t="shared" ref="H21:H22" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v/>
+      </c>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="34"/>
+      <c r="T21" s="34"/>
+      <c r="U21" s="34"/>
+      <c r="V21" s="34"/>
+      <c r="W21" s="34"/>
+      <c r="X21" s="34"/>
+      <c r="Y21" s="34"/>
+      <c r="Z21" s="34"/>
+      <c r="AA21" s="34"/>
+      <c r="AB21" s="34"/>
+      <c r="AC21" s="34"/>
+      <c r="AD21" s="34"/>
+      <c r="AE21" s="34"/>
+      <c r="AF21" s="34"/>
+      <c r="AG21" s="34"/>
+      <c r="AH21" s="34"/>
+      <c r="AI21" s="34"/>
+      <c r="AJ21" s="34"/>
+      <c r="AK21" s="34"/>
+      <c r="AL21" s="34"/>
+      <c r="AM21" s="34"/>
+      <c r="AN21" s="34"/>
+      <c r="AO21" s="34"/>
+      <c r="AP21" s="34"/>
+      <c r="AQ21" s="34"/>
+      <c r="AR21" s="34"/>
+      <c r="AS21" s="34"/>
+      <c r="AT21" s="34"/>
+      <c r="AU21" s="34"/>
+      <c r="AV21" s="34"/>
+      <c r="AW21" s="34"/>
+      <c r="AX21" s="34"/>
+      <c r="AY21" s="34"/>
+      <c r="AZ21" s="34"/>
+      <c r="BA21" s="34"/>
+      <c r="BB21" s="34"/>
+      <c r="BC21" s="34"/>
+      <c r="BD21" s="34"/>
+      <c r="BE21" s="34"/>
+      <c r="BF21" s="34"/>
+      <c r="BG21" s="34"/>
+      <c r="BH21" s="34"/>
+      <c r="BI21" s="34"/>
+      <c r="BJ21" s="34"/>
+      <c r="BK21" s="34"/>
+      <c r="BL21" s="34"/>
+    </row>
+    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B22" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33" t="str">
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="36"/>
-      <c r="R21" s="36"/>
-      <c r="S21" s="36"/>
-      <c r="T21" s="36"/>
-      <c r="U21" s="36"/>
-      <c r="V21" s="36"/>
-      <c r="W21" s="36"/>
-      <c r="X21" s="36"/>
-      <c r="Y21" s="36"/>
-      <c r="Z21" s="36"/>
-      <c r="AA21" s="36"/>
-      <c r="AB21" s="36"/>
-      <c r="AC21" s="36"/>
-      <c r="AD21" s="36"/>
-      <c r="AE21" s="36"/>
-      <c r="AF21" s="36"/>
-      <c r="AG21" s="36"/>
-      <c r="AH21" s="36"/>
-      <c r="AI21" s="36"/>
-      <c r="AJ21" s="36"/>
-      <c r="AK21" s="36"/>
-      <c r="AL21" s="36"/>
-      <c r="AM21" s="36"/>
-      <c r="AN21" s="36"/>
-      <c r="AO21" s="36"/>
-      <c r="AP21" s="36"/>
-      <c r="AQ21" s="36"/>
-      <c r="AR21" s="36"/>
-      <c r="AS21" s="36"/>
-      <c r="AT21" s="36"/>
-      <c r="AU21" s="36"/>
-      <c r="AV21" s="36"/>
-      <c r="AW21" s="36"/>
-      <c r="AX21" s="36"/>
-      <c r="AY21" s="36"/>
-      <c r="AZ21" s="36"/>
-      <c r="BA21" s="36"/>
-      <c r="BB21" s="36"/>
-      <c r="BC21" s="36"/>
-      <c r="BD21" s="36"/>
-      <c r="BE21" s="36"/>
-      <c r="BF21" s="36"/>
-      <c r="BG21" s="36"/>
-      <c r="BH21" s="36"/>
-      <c r="BI21" s="36"/>
-      <c r="BJ21" s="36"/>
-      <c r="BK21" s="36"/>
-      <c r="BL21" s="36"/>
-    </row>
-    <row r="22" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G22" s="6"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="36"/>
+      <c r="U22" s="36"/>
+      <c r="V22" s="36"/>
+      <c r="W22" s="36"/>
+      <c r="X22" s="36"/>
+      <c r="Y22" s="36"/>
+      <c r="Z22" s="36"/>
+      <c r="AA22" s="36"/>
+      <c r="AB22" s="36"/>
+      <c r="AC22" s="36"/>
+      <c r="AD22" s="36"/>
+      <c r="AE22" s="36"/>
+      <c r="AF22" s="36"/>
+      <c r="AG22" s="36"/>
+      <c r="AH22" s="36"/>
+      <c r="AI22" s="36"/>
+      <c r="AJ22" s="36"/>
+      <c r="AK22" s="36"/>
+      <c r="AL22" s="36"/>
+      <c r="AM22" s="36"/>
+      <c r="AN22" s="36"/>
+      <c r="AO22" s="36"/>
+      <c r="AP22" s="36"/>
+      <c r="AQ22" s="36"/>
+      <c r="AR22" s="36"/>
+      <c r="AS22" s="36"/>
+      <c r="AT22" s="36"/>
+      <c r="AU22" s="36"/>
+      <c r="AV22" s="36"/>
+      <c r="AW22" s="36"/>
+      <c r="AX22" s="36"/>
+      <c r="AY22" s="36"/>
+      <c r="AZ22" s="36"/>
+      <c r="BA22" s="36"/>
+      <c r="BB22" s="36"/>
+      <c r="BC22" s="36"/>
+      <c r="BD22" s="36"/>
+      <c r="BE22" s="36"/>
+      <c r="BF22" s="36"/>
+      <c r="BG22" s="36"/>
+      <c r="BH22" s="36"/>
+      <c r="BI22" s="36"/>
+      <c r="BJ22" s="36"/>
+      <c r="BK22" s="36"/>
+      <c r="BL22" s="36"/>
     </row>
     <row r="23" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="14"/>
-      <c r="F23" s="50"/>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="15"/>
+      <c r="C24" s="14"/>
+      <c r="F24" s="50"/>
+    </row>
+    <row r="25" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -3145,13 +3243,8 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D21">
+  <conditionalFormatting sqref="D7:D22">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3165,12 +3258,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL21">
+  <conditionalFormatting sqref="I5:BL22">
     <cfRule type="expression" dxfId="2" priority="33">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL21">
+  <conditionalFormatting sqref="I7:BL22">
     <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -3205,7 +3298,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D21</xm:sqref>
+          <xm:sqref>D7:D22</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Added the conversion between Celsius and Fahrenheit (#3)
</commit_message>
<xml_diff>
--- a/Documentation/Gantt_Chart.xlsx
+++ b/Documentation/Gantt_Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{648BC33F-75AD-4593-AFAD-B4B02218F8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45BA945-A4C5-44A1-9892-51A5103686AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>Task 4</t>
   </si>
@@ -213,9 +213,6 @@
     <t>Brenden</t>
   </si>
   <si>
-    <t>Basic CSS addition</t>
-  </si>
-  <si>
     <t>Mid Lab Check-off</t>
   </si>
   <si>
@@ -250,6 +247,21 @@
   </si>
   <si>
     <t>3 hours</t>
+  </si>
+  <si>
+    <t>Conversion Between F/C</t>
+  </si>
+  <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>2.2 hours</t>
+  </si>
+  <si>
+    <t>CSS on HTML Page</t>
+  </si>
+  <si>
+    <t>Next Task</t>
   </si>
 </sst>
 </file>
@@ -824,6 +836,18 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="12">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -831,18 +855,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1409,11 +1421,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL24"/>
+  <dimension ref="A1:BL25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1435,7 +1447,7 @@
         <v>29</v>
       </c>
       <c r="B1" s="53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1449,7 +1461,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I2" s="51"/>
     </row>
@@ -1458,119 +1470,119 @@
         <v>30</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="73">
+      <c r="D3" s="72"/>
+      <c r="E3" s="70">
         <v>44439</v>
       </c>
-      <c r="F3" s="73"/>
+      <c r="F3" s="70"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="72"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="70">
+      <c r="I4" s="67">
         <f>I5</f>
         <v>44438</v>
       </c>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="71"/>
-      <c r="N4" s="71"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="70">
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="67">
         <f>P5</f>
         <v>44445</v>
       </c>
-      <c r="Q4" s="71"/>
-      <c r="R4" s="71"/>
-      <c r="S4" s="71"/>
-      <c r="T4" s="71"/>
-      <c r="U4" s="71"/>
-      <c r="V4" s="72"/>
-      <c r="W4" s="70">
+      <c r="Q4" s="68"/>
+      <c r="R4" s="68"/>
+      <c r="S4" s="68"/>
+      <c r="T4" s="68"/>
+      <c r="U4" s="68"/>
+      <c r="V4" s="69"/>
+      <c r="W4" s="67">
         <f>W5</f>
         <v>44452</v>
       </c>
-      <c r="X4" s="71"/>
-      <c r="Y4" s="71"/>
-      <c r="Z4" s="71"/>
-      <c r="AA4" s="71"/>
-      <c r="AB4" s="71"/>
-      <c r="AC4" s="72"/>
-      <c r="AD4" s="70">
+      <c r="X4" s="68"/>
+      <c r="Y4" s="68"/>
+      <c r="Z4" s="68"/>
+      <c r="AA4" s="68"/>
+      <c r="AB4" s="68"/>
+      <c r="AC4" s="69"/>
+      <c r="AD4" s="67">
         <f>AD5</f>
         <v>44459</v>
       </c>
-      <c r="AE4" s="71"/>
-      <c r="AF4" s="71"/>
-      <c r="AG4" s="71"/>
-      <c r="AH4" s="71"/>
-      <c r="AI4" s="71"/>
-      <c r="AJ4" s="72"/>
-      <c r="AK4" s="70">
+      <c r="AE4" s="68"/>
+      <c r="AF4" s="68"/>
+      <c r="AG4" s="68"/>
+      <c r="AH4" s="68"/>
+      <c r="AI4" s="68"/>
+      <c r="AJ4" s="69"/>
+      <c r="AK4" s="67">
         <f>AK5</f>
         <v>44466</v>
       </c>
-      <c r="AL4" s="71"/>
-      <c r="AM4" s="71"/>
-      <c r="AN4" s="71"/>
-      <c r="AO4" s="71"/>
-      <c r="AP4" s="71"/>
-      <c r="AQ4" s="72"/>
-      <c r="AR4" s="70">
+      <c r="AL4" s="68"/>
+      <c r="AM4" s="68"/>
+      <c r="AN4" s="68"/>
+      <c r="AO4" s="68"/>
+      <c r="AP4" s="68"/>
+      <c r="AQ4" s="69"/>
+      <c r="AR4" s="67">
         <f>AR5</f>
         <v>44473</v>
       </c>
-      <c r="AS4" s="71"/>
-      <c r="AT4" s="71"/>
-      <c r="AU4" s="71"/>
-      <c r="AV4" s="71"/>
-      <c r="AW4" s="71"/>
-      <c r="AX4" s="72"/>
-      <c r="AY4" s="70">
+      <c r="AS4" s="68"/>
+      <c r="AT4" s="68"/>
+      <c r="AU4" s="68"/>
+      <c r="AV4" s="68"/>
+      <c r="AW4" s="68"/>
+      <c r="AX4" s="69"/>
+      <c r="AY4" s="67">
         <f>AY5</f>
         <v>44480</v>
       </c>
-      <c r="AZ4" s="71"/>
-      <c r="BA4" s="71"/>
-      <c r="BB4" s="71"/>
-      <c r="BC4" s="71"/>
-      <c r="BD4" s="71"/>
-      <c r="BE4" s="72"/>
-      <c r="BF4" s="70">
+      <c r="AZ4" s="68"/>
+      <c r="BA4" s="68"/>
+      <c r="BB4" s="68"/>
+      <c r="BC4" s="68"/>
+      <c r="BD4" s="68"/>
+      <c r="BE4" s="69"/>
+      <c r="BF4" s="67">
         <f>BF5</f>
         <v>44487</v>
       </c>
-      <c r="BG4" s="71"/>
-      <c r="BH4" s="71"/>
-      <c r="BI4" s="71"/>
-      <c r="BJ4" s="71"/>
-      <c r="BK4" s="71"/>
-      <c r="BL4" s="72"/>
+      <c r="BG4" s="68"/>
+      <c r="BH4" s="68"/>
+      <c r="BI4" s="68"/>
+      <c r="BJ4" s="68"/>
+      <c r="BK4" s="68"/>
+      <c r="BL4" s="69"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44438</v>
@@ -1816,10 +1828,10 @@
         <v>8</v>
       </c>
       <c r="G6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="I6" s="13" t="str">
         <f t="shared" ref="I6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
@@ -2118,7 +2130,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="59"/>
       <c r="D8" s="19"/>
@@ -2204,10 +2216,10 @@
         <v>44448</v>
       </c>
       <c r="G9" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="56" t="s">
         <v>52</v>
-      </c>
-      <c r="H9" s="56" t="s">
-        <v>53</v>
       </c>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
@@ -2288,10 +2300,10 @@
         <v>44450</v>
       </c>
       <c r="G10" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H10" s="56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
@@ -2370,10 +2382,10 @@
         <v>44451</v>
       </c>
       <c r="G11" s="56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H11" s="56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
@@ -2435,24 +2447,28 @@
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="48"/>
       <c r="B12" s="64" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C12" s="60" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="56">
         <f>F11</f>
         <v>44451</v>
       </c>
       <c r="F12" s="56">
-        <f>E12+1</f>
-        <v>44452</v>
-      </c>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
+        <f>E12</f>
+        <v>44451</v>
+      </c>
+      <c r="G12" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="56" t="s">
+        <v>58</v>
+      </c>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
       <c r="K12" s="34"/>
@@ -2513,12 +2529,21 @@
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="48"/>
       <c r="B13" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="60"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
+        <v>59</v>
+      </c>
+      <c r="C13" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="E13" s="56">
+        <v>44451</v>
+      </c>
+      <c r="F13" s="56">
+        <f>E13</f>
+        <v>44451</v>
+      </c>
       <c r="G13" s="56"/>
       <c r="H13" s="56"/>
       <c r="I13" s="34"/>
@@ -2579,18 +2604,16 @@
       <c r="BL13" s="34"/>
     </row>
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="61"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="60"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
       <c r="K14" s="34"/>
@@ -2649,14 +2672,18 @@
       <c r="BL14" s="34"/>
     </row>
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="49"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
+      <c r="A15" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="61"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
@@ -2715,7 +2742,7 @@
       <c r="BL15" s="34"/>
     </row>
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="48"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="65"/>
       <c r="C16" s="62"/>
       <c r="D16" s="27"/>
@@ -2735,8 +2762,8 @@
       <c r="R16" s="34"/>
       <c r="S16" s="34"/>
       <c r="T16" s="34"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
+      <c r="U16" s="34"/>
+      <c r="V16" s="34"/>
       <c r="W16" s="34"/>
       <c r="X16" s="34"/>
       <c r="Y16" s="34"/>
@@ -2801,8 +2828,8 @@
       <c r="R17" s="34"/>
       <c r="S17" s="34"/>
       <c r="T17" s="34"/>
-      <c r="U17" s="34"/>
-      <c r="V17" s="34"/>
+      <c r="U17" s="35"/>
+      <c r="V17" s="35"/>
       <c r="W17" s="34"/>
       <c r="X17" s="34"/>
       <c r="Y17" s="34"/>
@@ -2848,9 +2875,7 @@
     </row>
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="48"/>
-      <c r="B18" s="65" t="s">
-        <v>0</v>
-      </c>
+      <c r="B18" s="65"/>
       <c r="C18" s="62"/>
       <c r="D18" s="27"/>
       <c r="E18" s="57"/>
@@ -2873,7 +2898,7 @@
       <c r="V18" s="34"/>
       <c r="W18" s="34"/>
       <c r="X18" s="34"/>
-      <c r="Y18" s="35"/>
+      <c r="Y18" s="34"/>
       <c r="Z18" s="34"/>
       <c r="AA18" s="34"/>
       <c r="AB18" s="34"/>
@@ -2917,7 +2942,7 @@
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="48"/>
       <c r="B19" s="65" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="62"/>
       <c r="D19" s="27"/>
@@ -2941,7 +2966,7 @@
       <c r="V19" s="34"/>
       <c r="W19" s="34"/>
       <c r="X19" s="34"/>
-      <c r="Y19" s="34"/>
+      <c r="Y19" s="35"/>
       <c r="Z19" s="34"/>
       <c r="AA19" s="34"/>
       <c r="AB19" s="34"/>
@@ -2983,19 +3008,16 @@
       <c r="BL19" s="34"/>
     </row>
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="66"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17" t="str">
-        <f t="shared" ref="H8:H21" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v/>
-      </c>
+      <c r="A20" s="48"/>
+      <c r="B20" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="62"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
       <c r="K20" s="34"/>
@@ -3054,90 +3076,166 @@
       <c r="BL20" s="34"/>
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="66"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17" t="str">
+        <f t="shared" ref="H21:H22" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v/>
+      </c>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="34"/>
+      <c r="T21" s="34"/>
+      <c r="U21" s="34"/>
+      <c r="V21" s="34"/>
+      <c r="W21" s="34"/>
+      <c r="X21" s="34"/>
+      <c r="Y21" s="34"/>
+      <c r="Z21" s="34"/>
+      <c r="AA21" s="34"/>
+      <c r="AB21" s="34"/>
+      <c r="AC21" s="34"/>
+      <c r="AD21" s="34"/>
+      <c r="AE21" s="34"/>
+      <c r="AF21" s="34"/>
+      <c r="AG21" s="34"/>
+      <c r="AH21" s="34"/>
+      <c r="AI21" s="34"/>
+      <c r="AJ21" s="34"/>
+      <c r="AK21" s="34"/>
+      <c r="AL21" s="34"/>
+      <c r="AM21" s="34"/>
+      <c r="AN21" s="34"/>
+      <c r="AO21" s="34"/>
+      <c r="AP21" s="34"/>
+      <c r="AQ21" s="34"/>
+      <c r="AR21" s="34"/>
+      <c r="AS21" s="34"/>
+      <c r="AT21" s="34"/>
+      <c r="AU21" s="34"/>
+      <c r="AV21" s="34"/>
+      <c r="AW21" s="34"/>
+      <c r="AX21" s="34"/>
+      <c r="AY21" s="34"/>
+      <c r="AZ21" s="34"/>
+      <c r="BA21" s="34"/>
+      <c r="BB21" s="34"/>
+      <c r="BC21" s="34"/>
+      <c r="BD21" s="34"/>
+      <c r="BE21" s="34"/>
+      <c r="BF21" s="34"/>
+      <c r="BG21" s="34"/>
+      <c r="BH21" s="34"/>
+      <c r="BI21" s="34"/>
+      <c r="BJ21" s="34"/>
+      <c r="BK21" s="34"/>
+      <c r="BL21" s="34"/>
+    </row>
+    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B22" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33" t="str">
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="36"/>
-      <c r="R21" s="36"/>
-      <c r="S21" s="36"/>
-      <c r="T21" s="36"/>
-      <c r="U21" s="36"/>
-      <c r="V21" s="36"/>
-      <c r="W21" s="36"/>
-      <c r="X21" s="36"/>
-      <c r="Y21" s="36"/>
-      <c r="Z21" s="36"/>
-      <c r="AA21" s="36"/>
-      <c r="AB21" s="36"/>
-      <c r="AC21" s="36"/>
-      <c r="AD21" s="36"/>
-      <c r="AE21" s="36"/>
-      <c r="AF21" s="36"/>
-      <c r="AG21" s="36"/>
-      <c r="AH21" s="36"/>
-      <c r="AI21" s="36"/>
-      <c r="AJ21" s="36"/>
-      <c r="AK21" s="36"/>
-      <c r="AL21" s="36"/>
-      <c r="AM21" s="36"/>
-      <c r="AN21" s="36"/>
-      <c r="AO21" s="36"/>
-      <c r="AP21" s="36"/>
-      <c r="AQ21" s="36"/>
-      <c r="AR21" s="36"/>
-      <c r="AS21" s="36"/>
-      <c r="AT21" s="36"/>
-      <c r="AU21" s="36"/>
-      <c r="AV21" s="36"/>
-      <c r="AW21" s="36"/>
-      <c r="AX21" s="36"/>
-      <c r="AY21" s="36"/>
-      <c r="AZ21" s="36"/>
-      <c r="BA21" s="36"/>
-      <c r="BB21" s="36"/>
-      <c r="BC21" s="36"/>
-      <c r="BD21" s="36"/>
-      <c r="BE21" s="36"/>
-      <c r="BF21" s="36"/>
-      <c r="BG21" s="36"/>
-      <c r="BH21" s="36"/>
-      <c r="BI21" s="36"/>
-      <c r="BJ21" s="36"/>
-      <c r="BK21" s="36"/>
-      <c r="BL21" s="36"/>
-    </row>
-    <row r="22" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G22" s="6"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="36"/>
+      <c r="U22" s="36"/>
+      <c r="V22" s="36"/>
+      <c r="W22" s="36"/>
+      <c r="X22" s="36"/>
+      <c r="Y22" s="36"/>
+      <c r="Z22" s="36"/>
+      <c r="AA22" s="36"/>
+      <c r="AB22" s="36"/>
+      <c r="AC22" s="36"/>
+      <c r="AD22" s="36"/>
+      <c r="AE22" s="36"/>
+      <c r="AF22" s="36"/>
+      <c r="AG22" s="36"/>
+      <c r="AH22" s="36"/>
+      <c r="AI22" s="36"/>
+      <c r="AJ22" s="36"/>
+      <c r="AK22" s="36"/>
+      <c r="AL22" s="36"/>
+      <c r="AM22" s="36"/>
+      <c r="AN22" s="36"/>
+      <c r="AO22" s="36"/>
+      <c r="AP22" s="36"/>
+      <c r="AQ22" s="36"/>
+      <c r="AR22" s="36"/>
+      <c r="AS22" s="36"/>
+      <c r="AT22" s="36"/>
+      <c r="AU22" s="36"/>
+      <c r="AV22" s="36"/>
+      <c r="AW22" s="36"/>
+      <c r="AX22" s="36"/>
+      <c r="AY22" s="36"/>
+      <c r="AZ22" s="36"/>
+      <c r="BA22" s="36"/>
+      <c r="BB22" s="36"/>
+      <c r="BC22" s="36"/>
+      <c r="BD22" s="36"/>
+      <c r="BE22" s="36"/>
+      <c r="BF22" s="36"/>
+      <c r="BG22" s="36"/>
+      <c r="BH22" s="36"/>
+      <c r="BI22" s="36"/>
+      <c r="BJ22" s="36"/>
+      <c r="BK22" s="36"/>
+      <c r="BL22" s="36"/>
     </row>
     <row r="23" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="14"/>
-      <c r="F23" s="50"/>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="15"/>
+      <c r="C24" s="14"/>
+      <c r="F24" s="50"/>
+    </row>
+    <row r="25" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -3145,13 +3243,8 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D21">
+  <conditionalFormatting sqref="D7:D22">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3165,12 +3258,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL21">
+  <conditionalFormatting sqref="I5:BL22">
     <cfRule type="expression" dxfId="2" priority="33">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL21">
+  <conditionalFormatting sqref="I7:BL22">
     <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -3205,7 +3298,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D21</xm:sqref>
+          <xm:sqref>D7:D22</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
final final commit! PROJECT DONE
</commit_message>
<xml_diff>
--- a/Documentation/Gantt_Chart.xlsx
+++ b/Documentation/Gantt_Chart.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45BA945-A4C5-44A1-9892-51A5103686AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4710CA2-78E3-42C1-A0EA-A114F493D436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,13 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
-  <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 5</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -207,9 +201,6 @@
     <t>Henry</t>
   </si>
   <si>
-    <t>DTO Object</t>
-  </si>
-  <si>
     <t>Brenden</t>
   </si>
   <si>
@@ -261,7 +252,49 @@
     <t>CSS on HTML Page</t>
   </si>
   <si>
-    <t>Next Task</t>
+    <t>Place design into box</t>
+  </si>
+  <si>
+    <t>Backend RaspPI program</t>
+  </si>
+  <si>
+    <t>48 hours</t>
+  </si>
+  <si>
+    <t>60 hours</t>
+  </si>
+  <si>
+    <t>Database setup</t>
+  </si>
+  <si>
+    <t>Brendan/Matt</t>
+  </si>
+  <si>
+    <t>5.5 hours</t>
+  </si>
+  <si>
+    <t>Solder to 2m cable/ connections</t>
+  </si>
+  <si>
+    <t>1 hours</t>
+  </si>
+  <si>
+    <t>1.5 hours</t>
+  </si>
+  <si>
+    <t>Finish front end</t>
+  </si>
+  <si>
+    <t>Brenden/Brendan</t>
+  </si>
+  <si>
+    <t>20 hours</t>
+  </si>
+  <si>
+    <t>15 hours</t>
+  </si>
+  <si>
+    <t>DTO Object Controller</t>
   </si>
 </sst>
 </file>
@@ -836,6 +869,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="12">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -848,13 +888,6 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1424,15 +1457,15 @@
   <dimension ref="A1:BL25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
+      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="48" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.88671875" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.44140625" style="5" customWidth="1"/>
     <col min="6" max="6" width="10.44140625" customWidth="1"/>
@@ -1444,10 +1477,10 @@
   <sheetData>
     <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="49" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="53" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1458,131 +1491,131 @@
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="48" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I2" s="51"/>
     </row>
     <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="48" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="71" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="70">
+        <v>45</v>
+      </c>
+      <c r="C3" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="68"/>
+      <c r="E3" s="73">
         <v>44439</v>
       </c>
-      <c r="F3" s="70"/>
+      <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="71" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="72"/>
+        <v>29</v>
+      </c>
+      <c r="C4" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="68"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="67">
+      <c r="I4" s="70">
         <f>I5</f>
         <v>44438</v>
       </c>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="68"/>
-      <c r="M4" s="68"/>
-      <c r="N4" s="68"/>
-      <c r="O4" s="69"/>
-      <c r="P4" s="67">
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71"/>
+      <c r="M4" s="71"/>
+      <c r="N4" s="71"/>
+      <c r="O4" s="72"/>
+      <c r="P4" s="70">
         <f>P5</f>
         <v>44445</v>
       </c>
-      <c r="Q4" s="68"/>
-      <c r="R4" s="68"/>
-      <c r="S4" s="68"/>
-      <c r="T4" s="68"/>
-      <c r="U4" s="68"/>
-      <c r="V4" s="69"/>
-      <c r="W4" s="67">
+      <c r="Q4" s="71"/>
+      <c r="R4" s="71"/>
+      <c r="S4" s="71"/>
+      <c r="T4" s="71"/>
+      <c r="U4" s="71"/>
+      <c r="V4" s="72"/>
+      <c r="W4" s="70">
         <f>W5</f>
         <v>44452</v>
       </c>
-      <c r="X4" s="68"/>
-      <c r="Y4" s="68"/>
-      <c r="Z4" s="68"/>
-      <c r="AA4" s="68"/>
-      <c r="AB4" s="68"/>
-      <c r="AC4" s="69"/>
-      <c r="AD4" s="67">
+      <c r="X4" s="71"/>
+      <c r="Y4" s="71"/>
+      <c r="Z4" s="71"/>
+      <c r="AA4" s="71"/>
+      <c r="AB4" s="71"/>
+      <c r="AC4" s="72"/>
+      <c r="AD4" s="70">
         <f>AD5</f>
         <v>44459</v>
       </c>
-      <c r="AE4" s="68"/>
-      <c r="AF4" s="68"/>
-      <c r="AG4" s="68"/>
-      <c r="AH4" s="68"/>
-      <c r="AI4" s="68"/>
-      <c r="AJ4" s="69"/>
-      <c r="AK4" s="67">
+      <c r="AE4" s="71"/>
+      <c r="AF4" s="71"/>
+      <c r="AG4" s="71"/>
+      <c r="AH4" s="71"/>
+      <c r="AI4" s="71"/>
+      <c r="AJ4" s="72"/>
+      <c r="AK4" s="70">
         <f>AK5</f>
         <v>44466</v>
       </c>
-      <c r="AL4" s="68"/>
-      <c r="AM4" s="68"/>
-      <c r="AN4" s="68"/>
-      <c r="AO4" s="68"/>
-      <c r="AP4" s="68"/>
-      <c r="AQ4" s="69"/>
-      <c r="AR4" s="67">
+      <c r="AL4" s="71"/>
+      <c r="AM4" s="71"/>
+      <c r="AN4" s="71"/>
+      <c r="AO4" s="71"/>
+      <c r="AP4" s="71"/>
+      <c r="AQ4" s="72"/>
+      <c r="AR4" s="70">
         <f>AR5</f>
         <v>44473</v>
       </c>
-      <c r="AS4" s="68"/>
-      <c r="AT4" s="68"/>
-      <c r="AU4" s="68"/>
-      <c r="AV4" s="68"/>
-      <c r="AW4" s="68"/>
-      <c r="AX4" s="69"/>
-      <c r="AY4" s="67">
+      <c r="AS4" s="71"/>
+      <c r="AT4" s="71"/>
+      <c r="AU4" s="71"/>
+      <c r="AV4" s="71"/>
+      <c r="AW4" s="71"/>
+      <c r="AX4" s="72"/>
+      <c r="AY4" s="70">
         <f>AY5</f>
         <v>44480</v>
       </c>
-      <c r="AZ4" s="68"/>
-      <c r="BA4" s="68"/>
-      <c r="BB4" s="68"/>
-      <c r="BC4" s="68"/>
-      <c r="BD4" s="68"/>
-      <c r="BE4" s="69"/>
-      <c r="BF4" s="67">
+      <c r="AZ4" s="71"/>
+      <c r="BA4" s="71"/>
+      <c r="BB4" s="71"/>
+      <c r="BC4" s="71"/>
+      <c r="BD4" s="71"/>
+      <c r="BE4" s="72"/>
+      <c r="BF4" s="70">
         <f>BF5</f>
         <v>44487</v>
       </c>
-      <c r="BG4" s="68"/>
-      <c r="BH4" s="68"/>
-      <c r="BI4" s="68"/>
-      <c r="BJ4" s="68"/>
-      <c r="BK4" s="68"/>
-      <c r="BL4" s="69"/>
+      <c r="BG4" s="71"/>
+      <c r="BH4" s="71"/>
+      <c r="BI4" s="71"/>
+      <c r="BJ4" s="71"/>
+      <c r="BK4" s="71"/>
+      <c r="BL4" s="72"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
+        <v>30</v>
+      </c>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44438</v>
@@ -1810,28 +1843,28 @@
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="49" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="F6" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I6" s="13" t="str">
         <f t="shared" ref="I6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
@@ -2060,7 +2093,7 @@
     </row>
     <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="52"/>
       <c r="E7"/>
@@ -2127,10 +2160,10 @@
     </row>
     <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="49" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8" s="59"/>
       <c r="D8" s="19"/>
@@ -2197,13 +2230,13 @@
     </row>
     <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="49" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="64" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C9" s="60" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D9" s="22">
         <v>1</v>
@@ -2216,10 +2249,10 @@
         <v>44448</v>
       </c>
       <c r="G9" s="56" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H9" s="56" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
@@ -2280,16 +2313,16 @@
     </row>
     <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="49" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B10" s="64" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D10" s="22">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E10" s="56">
         <f>F9</f>
@@ -2300,10 +2333,10 @@
         <v>44450</v>
       </c>
       <c r="G10" s="56" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H10" s="56" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
@@ -2365,10 +2398,10 @@
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="48"/>
       <c r="B11" s="64" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="C11" s="60" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D11" s="22">
         <v>1</v>
@@ -2382,10 +2415,10 @@
         <v>44451</v>
       </c>
       <c r="G11" s="56" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H11" s="56" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
@@ -2447,10 +2480,10 @@
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="48"/>
       <c r="B12" s="64" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C12" s="60" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D12" s="22">
         <v>1</v>
@@ -2464,10 +2497,10 @@
         <v>44451</v>
       </c>
       <c r="G12" s="56" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H12" s="56" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
@@ -2529,13 +2562,13 @@
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="48"/>
       <c r="B13" s="64" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C13" s="60" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D13" s="22">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="56">
         <v>44451</v>
@@ -2544,8 +2577,12 @@
         <f>E13</f>
         <v>44451</v>
       </c>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
+      <c r="G13" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="56" t="s">
+        <v>50</v>
+      </c>
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
       <c r="K13" s="34"/>
@@ -2605,9 +2642,7 @@
     </row>
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="48"/>
-      <c r="B14" s="64" t="s">
-        <v>60</v>
-      </c>
+      <c r="B14" s="64"/>
       <c r="C14" s="60"/>
       <c r="D14" s="22"/>
       <c r="E14" s="56"/>
@@ -2673,10 +2708,10 @@
     </row>
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="49" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C15" s="61"/>
       <c r="D15" s="24"/>
@@ -2743,13 +2778,27 @@
     </row>
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="49"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
+      <c r="B16" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="27">
+        <v>1</v>
+      </c>
+      <c r="E16" s="57">
+        <v>44465</v>
+      </c>
+      <c r="F16" s="57">
+        <v>44469</v>
+      </c>
+      <c r="G16" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="57" t="s">
+        <v>54</v>
+      </c>
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
@@ -2809,13 +2858,27 @@
     </row>
     <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="48"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
+      <c r="B17" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="27">
+        <v>1</v>
+      </c>
+      <c r="E17" s="57">
+        <v>44458</v>
+      </c>
+      <c r="F17" s="57">
+        <v>44468</v>
+      </c>
+      <c r="G17" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="57" t="s">
+        <v>60</v>
+      </c>
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
@@ -2875,13 +2938,27 @@
     </row>
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="48"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
+      <c r="B18" s="65" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="27">
+        <v>1</v>
+      </c>
+      <c r="E18" s="57">
+        <v>44467</v>
+      </c>
+      <c r="F18" s="57">
+        <v>44469</v>
+      </c>
+      <c r="G18" s="57" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="57" t="s">
+        <v>63</v>
+      </c>
       <c r="I18" s="34"/>
       <c r="J18" s="34"/>
       <c r="K18" s="34"/>
@@ -2942,14 +3019,26 @@
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="48"/>
       <c r="B19" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
+        <v>64</v>
+      </c>
+      <c r="C19" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="27">
+        <v>1</v>
+      </c>
+      <c r="E19" s="57">
+        <v>44469</v>
+      </c>
+      <c r="F19" s="57">
+        <v>44469</v>
+      </c>
+      <c r="G19" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="57" t="s">
+        <v>66</v>
+      </c>
       <c r="I19" s="34"/>
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
@@ -3010,14 +3099,26 @@
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="48"/>
       <c r="B20" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="27">
         <v>1</v>
       </c>
-      <c r="C20" s="62"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
+      <c r="E20" s="57">
+        <v>44467</v>
+      </c>
+      <c r="F20" s="57">
+        <v>44469</v>
+      </c>
+      <c r="G20" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="57" t="s">
+        <v>70</v>
+      </c>
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
       <c r="K20" s="34"/>
@@ -3077,7 +3178,7 @@
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="48" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" s="66"/>
       <c r="C21" s="63"/>
@@ -3148,10 +3249,10 @@
     </row>
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="49" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C22" s="29"/>
       <c r="D22" s="30"/>
@@ -3231,11 +3332,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -3243,6 +3339,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D22">
     <cfRule type="dataBar" priority="14">
@@ -3321,79 +3422,79 @@
     <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:2" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="39"/>
     </row>
     <row r="3" spans="1:2" s="44" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="45" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="45"/>
     </row>
     <row r="4" spans="1:2" s="41" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A4" s="42" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="43" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="42" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="38" customFormat="1" ht="204.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="41" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A8" s="42" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="43" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="38" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="46" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="41" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A11" s="42" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="43" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="38" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="46" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="41" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A14" s="42" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="43" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="43" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>